<commit_message>
refactor: migrate configuration from Python to YAML format
</commit_message>
<xml_diff>
--- a/batch/tasks_setting.xlsx
+++ b/batch/tasks_setting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="22140"/>
+    <workbookView windowWidth="15488" windowHeight="9317"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Video File</t>
   </si>
@@ -43,18 +43,41 @@
   <si>
     <t>Status</t>
   </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=U4aFbyzrTdc</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,12 +424,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -509,31 +547,20 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -542,124 +569,134 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -713,221 +750,7 @@
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="double">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
-  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
-    </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
-    </tableStyle>
-  </tableStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -937,9 +760,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="WPS">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -947,39 +770,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4874CB"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EE822F"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="F2BA02"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="75BD42"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="30C0B4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="E54C5E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0026E5"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="7E1FAD"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="WPS">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1011,7 +834,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1046,135 +868,171 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="WPS">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumOff val="17500"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
-              <a:schemeClr val="phClr"/>
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="2700000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:hueOff val="-2520000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
-              <a:schemeClr val="phClr"/>
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="2700000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:gradFill>
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:schemeClr val="phClr">
-                  <a:hueOff val="-4200000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="100000">
-                <a:schemeClr val="phClr"/>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="2700000" scaled="1"/>
-          </a:gradFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="101600" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:schemeClr val="phClr">
-                <a:alpha val="60000"/>
-              </a:schemeClr>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:reflection stA="50000" endA="300" endPos="40000" dist="25400" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1186,36 +1044,43 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="4"/>
-  <cols>
-    <col min="1" max="1" width="15.2211538461538" customWidth="1"/>
-    <col min="2" max="2" width="20.8269230769231" customWidth="1"/>
-    <col min="3" max="3" width="19.3846153846154" customWidth="1"/>
-    <col min="4" max="4" width="13.9326923076923" customWidth="1"/>
-    <col min="5" max="5" width="12.0192307692308" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" outlineLevelRow="1" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>